<commit_message>
Updated Distance Points Table
</commit_message>
<xml_diff>
--- a/DriveTemplateDevelopment.xlsx
+++ b/DriveTemplateDevelopment.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2fd3bccd6dbaea2b/GitGud/ExcelDriveSummary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="691" documentId="13_ncr:1_{F7269803-218D-4718-B04F-3CDC29A5C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84D186B0-BE98-4F65-A99B-8928868D591B}"/>
+  <xr:revisionPtr revIDLastSave="1192" documentId="13_ncr:1_{F7269803-218D-4718-B04F-3CDC29A5C001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{511AA5FF-C6DF-4ABD-B92E-69F4042ADEA5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{B12B6E18-E294-4985-A977-422328ADD677}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="69">
   <si>
     <t>End</t>
   </si>
@@ -236,9 +236,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Rem Distance Pts</t>
-  </si>
-  <si>
     <t>Night Extr or Calc</t>
   </si>
   <si>
@@ -249,6 +246,32 @@
   </si>
   <si>
     <t>Days Left</t>
+  </si>
+  <si>
+    <t>Last Month's Status</t>
+  </si>
+  <si>
+    <t>Distance Upper Limit</t>
+  </si>
+  <si>
+    <t>Legend</t>
+  </si>
+  <si>
+    <t>Manual Data</t>
+  </si>
+  <si>
+    <t>Config Data</t>
+  </si>
+  <si>
+    <t>The predicted status gives a realistic prediction of the driving status. 
+If the prediction is disable, best case scenario is assumed, which is 
+50 point drive days and the distance remains in the same bracket.</t>
+  </si>
+  <si>
+    <t>Rem Dist Points</t>
+  </si>
+  <si>
+    <t>Rem - Dist</t>
   </si>
 </sst>
 </file>
@@ -302,7 +325,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,8 +350,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -421,12 +456,58 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -545,10 +626,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -572,7 +653,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -580,8 +709,14 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="20">
     <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -596,13 +731,14 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
+        <right/>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -615,6 +751,203 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -628,25 +961,16 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
         <right style="thin">
           <color indexed="64"/>
         </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
+        <top/>
+        <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -707,7 +1031,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{6816E4B5-3A62-4F29-9CCF-2FA42321C8A7}">
-      <tableStyleElement type="wholeTable" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="19"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -739,16 +1063,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{34FD56D6-F605-4784-BB9F-783DF2FD6679}" name="NightTimeDrive5" displayName="NightTimeDrive5" ref="I6:J8" headerRowDxfId="6" dataDxfId="4" headerRowBorderDxfId="5">
-  <autoFilter ref="I6:J8" xr:uid="{76285C9C-3E4D-42C9-A22A-CEC4B871EA2B}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{932FCD99-6FCF-4AE6-A66E-74A568E6D121}" name="NightTimeDrive55" displayName="NightTimeDrive55" ref="I11:J13" headerRowDxfId="18" dataDxfId="12" headerRowBorderDxfId="17">
+  <autoFilter ref="I11:J13" xr:uid="{932FCD99-6FCF-4AE6-A66E-74A568E6D121}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{22A1BAEB-890B-47E5-BA99-B3BF4B1258DC}" name="Time" totalsRowLabel="Total" dataDxfId="3" totalsRowDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{EC1C7F3A-D38A-492B-910A-AF3CF9E33416}" name="Points" totalsRowFunction="sum" dataDxfId="1" totalsRowDxfId="0">
-      <calculatedColumnFormula>2*NightTimeDrive5[[#This Row],[Time]]</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{9EB75FFC-DA63-4FB2-9EDD-0F3F85DD3EDF}" name="Time" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{0F4B0F6D-D478-4EAB-BC51-738227841C7E}" name="Points" totalsRowFunction="sum" dataDxfId="13" totalsRowDxfId="15">
+      <calculatedColumnFormula>2*NightTimeDrive55[[#This Row],[Time]]</calculatedColumnFormula>
     </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E011F3DC-4D15-4380-B07D-61D2F4291EE8}" name="Table2" displayName="Table2" ref="O6:U13" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1" headerRowBorderDxfId="10" tableBorderDxfId="11" totalsRowBorderDxfId="9">
+  <autoFilter ref="O6:U13" xr:uid="{E011F3DC-4D15-4380-B07D-61D2F4291EE8}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{67CAC795-E571-47E4-824E-016D041A5D00}" name="Lower" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{582822E9-3DEB-4508-AA7B-DD7A6A2BB156}" name="Upper" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{003DDF9D-C1E4-4FD2-9601-690C9D687E6C}" name="Blue" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{14CD9C7F-BAB0-475F-BA55-23A1510F9B02}" name="Bronze" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{6E16B529-049D-4870-9F01-54E881E3AD80}" name="Silver" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{D851F32A-6D40-41EC-9D8C-3904177A2CC4}" name="Gold" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{F6586344-39BA-4E77-A4BF-62456CE19804}" name="Diamond" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1098,7 +1446,7 @@
       </c>
       <c r="C2" s="8">
         <f ca="1">IF(ROUND(DAY(EOMONTH(TODAY(),0))*AVERAGE(OFFSET(H2,0,0,COUNTA(H2:INDEX(H:H,DAY(EOMONTH(TODAY(),-1))+1)),1)),0)&gt;1500,1500,ROUND(DAY(EOMONTH(TODAY(),0))*AVERAGE(OFFSET(H2,0,0,COUNTA(H2:INDEX(H:H,DAY(EOMONTH(TODAY(),-1))+1)),1)),0))</f>
-        <v>1289</v>
+        <v>1500</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="7" t="s">
@@ -1144,7 +1492,7 @@
       </c>
       <c r="E3" s="10">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),1)</f>
-        <v>45689</v>
+        <v>45717</v>
       </c>
       <c r="F3" s="1" t="str">
         <f ca="1">TEXT(E3,"dddd")</f>
@@ -1187,7 +1535,7 @@
       </c>
       <c r="E4" s="10">
         <f ca="1">E3+1</f>
-        <v>45690</v>
+        <v>45718</v>
       </c>
       <c r="F4" s="1" t="str">
         <f t="shared" ref="F4:F30" ca="1" si="0">TEXT(E4,"dddd")</f>
@@ -1227,11 +1575,11 @@
       </c>
       <c r="C5" s="1">
         <f ca="1">VLOOKUP(DAY(EOMONTH(TODAY(),0))*AVERAGE(OFFSET(G2,0,0,COUNTA(G2:INDEX(G:G,DAY(EOMONTH(TODAY(),-1))+1)),1)),J2:L17,3,TRUE)</f>
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="E5" s="10">
         <f t="shared" ref="E5:E33" ca="1" si="1">E4+1</f>
-        <v>45691</v>
+        <v>45719</v>
       </c>
       <c r="F5" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1274,7 +1622,7 @@
       </c>
       <c r="E6" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45692</v>
+        <v>45720</v>
       </c>
       <c r="F6" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1314,12 +1662,12 @@
       </c>
       <c r="C7" s="8">
         <f ca="1">SUM(C2:C6)</f>
-        <v>2309</v>
+        <v>2480</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45693</v>
+        <v>45721</v>
       </c>
       <c r="F7" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1356,7 +1704,7 @@
     <row r="8" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E8" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45694</v>
+        <v>45722</v>
       </c>
       <c r="F8" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1389,7 +1737,7 @@
       </c>
       <c r="E9" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45695</v>
+        <v>45723</v>
       </c>
       <c r="F9" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1428,7 +1776,7 @@
       <c r="D10" s="14"/>
       <c r="E10" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45696</v>
+        <v>45724</v>
       </c>
       <c r="F10" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1466,7 +1814,7 @@
       <c r="D11" s="16"/>
       <c r="E11" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45697</v>
+        <v>45725</v>
       </c>
       <c r="F11" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1496,7 +1844,7 @@
     <row r="12" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E12" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45698</v>
+        <v>45726</v>
       </c>
       <c r="F12" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1527,7 +1875,7 @@
       <c r="C13" s="20"/>
       <c r="E13" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45699</v>
+        <v>45727</v>
       </c>
       <c r="F13" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1557,7 +1905,7 @@
     <row r="14" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E14" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45700</v>
+        <v>45728</v>
       </c>
       <c r="F14" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1588,7 +1936,7 @@
       <c r="C15" s="14"/>
       <c r="E15" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45701</v>
+        <v>45729</v>
       </c>
       <c r="F15" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1618,7 +1966,7 @@
     <row r="16" spans="2:20" x14ac:dyDescent="0.25">
       <c r="E16" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45702</v>
+        <v>45730</v>
       </c>
       <c r="F16" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1648,7 +1996,7 @@
       <c r="C17" s="3"/>
       <c r="E17" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45703</v>
+        <v>45731</v>
       </c>
       <c r="F17" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1679,7 +2027,7 @@
       <c r="B18" s="3"/>
       <c r="E18" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45704</v>
+        <v>45732</v>
       </c>
       <c r="F18" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1700,7 +2048,7 @@
     <row r="19" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E19" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45705</v>
+        <v>45733</v>
       </c>
       <c r="F19" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1721,7 +2069,7 @@
     <row r="20" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E20" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45706</v>
+        <v>45734</v>
       </c>
       <c r="F20" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1742,7 +2090,7 @@
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E21" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45707</v>
+        <v>45735</v>
       </c>
       <c r="F21" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1759,7 +2107,7 @@
     <row r="22" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E22" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45708</v>
+        <v>45736</v>
       </c>
       <c r="F22" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1777,7 +2125,7 @@
     <row r="23" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E23" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45709</v>
+        <v>45737</v>
       </c>
       <c r="F23" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1796,7 +2144,7 @@
       <c r="B24" s="2"/>
       <c r="E24" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45710</v>
+        <v>45738</v>
       </c>
       <c r="F24" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1815,7 +2163,7 @@
     <row r="25" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E25" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45711</v>
+        <v>45739</v>
       </c>
       <c r="F25" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1833,7 +2181,7 @@
     <row r="26" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E26" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45712</v>
+        <v>45740</v>
       </c>
       <c r="F26" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1851,7 +2199,7 @@
     <row r="27" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E27" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45713</v>
+        <v>45741</v>
       </c>
       <c r="F27" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1869,7 +2217,7 @@
     <row r="28" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E28" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45714</v>
+        <v>45742</v>
       </c>
       <c r="F28" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1887,7 +2235,7 @@
     <row r="29" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E29" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45715</v>
+        <v>45743</v>
       </c>
       <c r="F29" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1905,7 +2253,7 @@
     <row r="30" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E30" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45716</v>
+        <v>45744</v>
       </c>
       <c r="F30" s="1" t="str">
         <f t="shared" ca="1" si="0"/>
@@ -1922,7 +2270,7 @@
     <row r="31" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E31" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45717</v>
+        <v>45745</v>
       </c>
       <c r="F31" s="1" t="str">
         <f t="shared" ref="F31:F33" ca="1" si="2">TEXT(E31,"dddd")</f>
@@ -1939,7 +2287,7 @@
     <row r="32" spans="2:18" x14ac:dyDescent="0.25">
       <c r="E32" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45718</v>
+        <v>45746</v>
       </c>
       <c r="F32" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -1956,7 +2304,7 @@
     <row r="33" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E33" s="10">
         <f t="shared" ca="1" si="1"/>
-        <v>45719</v>
+        <v>45747</v>
       </c>
       <c r="F33" s="1" t="str">
         <f t="shared" ca="1" si="2"/>
@@ -2070,7 +2418,7 @@
     <row r="2" spans="2:22" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="48" t="str" cm="1">
         <f t="array" aca="1" ref="B2" ca="1">_xlfn.CONCAT("Drive Summary ", MID(CELL("filename",A1),FIND("]",CELL("filename",A1))+1,31), " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Develop February 2025</v>
+        <v>Drive Summary Develop March 2025</v>
       </c>
       <c r="C2" s="48"/>
       <c r="D2" s="48"/>
@@ -2092,12 +2440,12 @@
       </c>
       <c r="C5" s="25">
         <f ca="1">IF(IF($C$16,G7,G6+G13)&gt;1500, 1500, IF($C$16,G7,G6+G13))</f>
-        <v>898</v>
+        <v>1500</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>February 2025</v>
+        <v>March 2025</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>25</v>
@@ -2181,11 +2529,11 @@
       </c>
       <c r="F7" s="25">
         <f ca="1">F6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>413</v>
+        <v>1829</v>
       </c>
       <c r="G7" s="25">
         <f ca="1">G6/(DAY(TODAY())-1)*DAY(EOMONTH(TODAY(), 0))</f>
-        <v>814.33333333333326</v>
+        <v>3606.333333333333</v>
       </c>
       <c r="I7" s="1">
         <v>0</v>
@@ -2213,7 +2561,7 @@
       </c>
       <c r="T7" s="6">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>200</v>
+        <v>1250</v>
       </c>
       <c r="U7" s="9">
         <f>VLOOKUP(F6,I7:K21,2,TRUE)-F6</f>
@@ -2297,18 +2645,18 @@
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>1938</v>
+        <v>2540</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="24">
         <f ca="1">F6/(DAY(TODAY())-1)</f>
-        <v>14.75</v>
+        <v>59</v>
       </c>
       <c r="G10" s="24">
         <f ca="1">G6/(DAY(TODAY())-1)</f>
-        <v>29.083333333333332</v>
+        <v>116.33333333333333</v>
       </c>
       <c r="I10" s="1">
         <v>450</v>
@@ -2336,7 +2684,7 @@
       </c>
       <c r="T10" s="6" t="str">
         <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
-        <v>Silver</v>
+        <v>Diamond</v>
       </c>
     </row>
     <row r="11" spans="2:22" x14ac:dyDescent="0.25">
@@ -2369,7 +2717,7 @@
       </c>
       <c r="C12" s="1" t="str">
         <f ca="1">VLOOKUP(C10,M7:O11,3,TRUE)</f>
-        <v>Silver</v>
+        <v>Diamond</v>
       </c>
       <c r="D12" s="9"/>
       <c r="E12" s="26"/>
@@ -2394,7 +2742,7 @@
       </c>
       <c r="T12" s="6">
         <f ca="1">VLOOKUP(C10,M7:O11,1,TRUE)</f>
-        <v>1600</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="13" spans="2:22" x14ac:dyDescent="0.25">
@@ -2414,7 +2762,7 @@
       </c>
       <c r="G13" s="1">
         <f ca="1">50*(DAY(EOMONTH(TODAY(), 0))-DAY(TODAY()-1))</f>
-        <v>200</v>
+        <v>1250</v>
       </c>
       <c r="I13" s="1">
         <v>900</v>
@@ -2432,7 +2780,7 @@
       </c>
       <c r="T13" s="9">
         <f ca="1">C5+C6+C7+C9+C8</f>
-        <v>1938</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="14" spans="2:22" x14ac:dyDescent="0.25">
@@ -2479,7 +2827,7 @@
       </c>
       <c r="T15" s="9">
         <f ca="1">T13-T12</f>
-        <v>338</v>
+        <v>40</v>
       </c>
       <c r="U15" s="9"/>
     </row>
@@ -2509,11 +2857,11 @@
       </c>
       <c r="T16" s="6">
         <f ca="1">INT(T15/20)</f>
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="U16" s="6">
         <f ca="1">IF(T16=0,0,T16*150-1)</f>
-        <v>2399</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2544,7 +2892,7 @@
       </c>
       <c r="T17" s="6">
         <f ca="1">20*T16</f>
-        <v>320</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
@@ -2573,7 +2921,7 @@
       </c>
       <c r="T18" s="6">
         <f ca="1">MIN(300-T17,C8)</f>
-        <v>-20</v>
+        <v>260</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
@@ -2600,9 +2948,9 @@
       <c r="S19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="T19" s="6" t="e">
+      <c r="T19" s="6">
         <f ca="1">_xlfn.XLOOKUP(T18,K7:K21,J7:J21)</f>
-        <v>#N/A</v>
+        <v>449</v>
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
@@ -2647,9 +2995,9 @@
       <c r="S21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="T21" s="9" t="e">
+      <c r="T21" s="9">
         <f ca="1">T19-F6</f>
-        <v>#N/A</v>
+        <v>95</v>
       </c>
       <c r="U21" s="9"/>
     </row>
@@ -2661,9 +3009,9 @@
       <c r="S22" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="T22" s="9" t="e">
+      <c r="T22" s="9">
         <f ca="1">T21-F13</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="U22" s="9"/>
     </row>
@@ -2822,41 +3170,42 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:AB50"/>
+  <dimension ref="B2:AF50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.7109375" style="6" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="2.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="7" width="9.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" style="6" customWidth="1"/>
     <col min="8" max="8" width="2.7109375" style="6" customWidth="1"/>
-    <col min="9" max="10" width="9.42578125" style="6" customWidth="1"/>
+    <col min="9" max="10" width="9.7109375" style="6" customWidth="1"/>
     <col min="11" max="11" width="2.7109375" style="6" customWidth="1"/>
-    <col min="12" max="12" width="21.7109375" style="6" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="6" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="2.7109375" style="6" customWidth="1"/>
-    <col min="15" max="17" width="9.42578125" style="6" customWidth="1"/>
-    <col min="18" max="18" width="2.7109375" style="6" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" style="17" customWidth="1"/>
-    <col min="20" max="20" width="6.42578125" style="6" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="6.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="8.85546875" style="6"/>
-    <col min="25" max="25" width="8.85546875" style="6" customWidth="1"/>
-    <col min="26" max="16384" width="8.85546875" style="6"/>
+    <col min="15" max="20" width="9.7109375" style="6" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" style="6" customWidth="1"/>
+    <col min="22" max="22" width="2.7109375" style="6" customWidth="1"/>
+    <col min="23" max="23" width="9.7109375" style="17" customWidth="1"/>
+    <col min="24" max="26" width="9.7109375" style="6" customWidth="1"/>
+    <col min="27" max="27" width="8.85546875" style="6" customWidth="1"/>
+    <col min="28" max="28" width="8.85546875" style="6"/>
+    <col min="29" max="29" width="8.85546875" style="6" customWidth="1"/>
+    <col min="30" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="48" t="str">
-        <f ca="1">_xlfn.CONCAT("Drive Summary ", M12, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
-        <v>Drive Summary Stefan February 2025</v>
+        <f ca="1">_xlfn.CONCAT("Drive Summary ", M13, " ",TEXT(TODAY(), "mmmm yyyy"))</f>
+        <v>Drive Summary Stefan March 2025</v>
       </c>
       <c r="C2" s="48"/>
       <c r="D2" s="48"/>
@@ -2867,7 +3216,7 @@
       <c r="I2" s="48"/>
       <c r="J2" s="48"/>
     </row>
-    <row r="3" spans="2:28" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:32" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="48"/>
       <c r="C3" s="48"/>
       <c r="D3" s="48"/>
@@ -2878,18 +3227,18 @@
       <c r="I3" s="48"/>
       <c r="J3" s="48"/>
     </row>
-    <row r="5" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>23</v>
       </c>
       <c r="C5" s="25">
         <f ca="1">MIN(1500, IF($C$16,G7,G6+G13))</f>
-        <v>1438.25</v>
+        <v>1500</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="7" t="str">
         <f ca="1">TEXT(TODAY(), "mmmm yyyy")</f>
-        <v>February 2025</v>
+        <v>March 2025</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>25</v>
@@ -2898,7 +3247,7 @@
         <v>17</v>
       </c>
       <c r="I5" s="43" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="J5" s="44"/>
       <c r="L5" s="43" t="s">
@@ -2906,20 +3255,24 @@
       </c>
       <c r="M5" s="44"/>
       <c r="O5" s="43" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="P5" s="47"/>
-      <c r="Q5" s="44"/>
-      <c r="S5" s="43" t="s">
+      <c r="Q5" s="47"/>
+      <c r="R5" s="47"/>
+      <c r="S5" s="47"/>
+      <c r="T5" s="47"/>
+      <c r="U5" s="44"/>
+      <c r="W5" s="43" t="s">
         <v>38</v>
       </c>
-      <c r="T5" s="47"/>
-      <c r="U5" s="47"/>
-      <c r="V5" s="44"/>
-      <c r="AA5" s="46"/>
-      <c r="AB5" s="46"/>
-    </row>
-    <row r="6" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="X5" s="47"/>
+      <c r="Y5" s="47"/>
+      <c r="Z5" s="44"/>
+      <c r="AE5" s="46"/>
+      <c r="AF5" s="46"/>
+    </row>
+    <row r="6" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
@@ -2930,149 +3283,177 @@
         <v>27</v>
       </c>
       <c r="F6" s="30">
-        <v>261</v>
+        <v>484</v>
       </c>
       <c r="G6" s="23">
-        <v>1143</v>
-      </c>
-      <c r="I6" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="J6" s="7" t="s">
-        <v>17</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="I6" s="55" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="55"/>
       <c r="L6" s="39" t="s">
         <v>15</v>
       </c>
       <c r="M6" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="O6" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="P6" s="7" t="s">
+      <c r="P6" s="61" t="s">
         <v>18</v>
       </c>
-      <c r="Q6" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="S6" s="7" t="s">
+      <c r="Q6" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6" s="61" t="s">
+        <v>10</v>
+      </c>
+      <c r="S6" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="T6" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="U6" s="62" t="s">
+        <v>4</v>
+      </c>
+      <c r="W6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="T6" s="7" t="s">
+      <c r="X6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="U6" s="7" t="s">
+      <c r="Y6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="V6" s="7" t="s">
+      <c r="Z6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="Z6"/>
-      <c r="AA6" s="33"/>
-      <c r="AB6" s="33"/>
-    </row>
-    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AD6"/>
+      <c r="AE6" s="33"/>
+      <c r="AF6" s="33"/>
+    </row>
+    <row r="7" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="42">
-        <f>IF( AND( M8&lt;=M14+M15, M8&gt;=M14-M15 ), M8, M14)</f>
-        <v>248</v>
+      <c r="C7" s="41">
+        <f>IF( AND( M8&lt;=M15+M14, M8&gt;=M15-M14 ), M8, M15)</f>
+        <v>300</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F7" s="25">
-        <f ca="1">F6/M18*M17</f>
-        <v>304.5</v>
+        <f ca="1">F6/M19*M18</f>
+        <v>2500.666666666667</v>
       </c>
       <c r="G7" s="25">
-        <f ca="1">G6/M18*M17</f>
-        <v>1333.5</v>
-      </c>
-      <c r="I7" s="1">
-        <v>23</v>
-      </c>
-      <c r="J7" s="1">
-        <f>2*NightTimeDrive5[[#This Row],[Time]]</f>
-        <v>46</v>
-      </c>
+        <f ca="1">G6/M19*M18</f>
+        <v>1550</v>
+      </c>
+      <c r="I7" s="56" t="s">
+        <v>64</v>
+      </c>
+      <c r="J7" s="56"/>
       <c r="L7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="M7" s="37">
         <v>300</v>
       </c>
-      <c r="O7" s="1">
+      <c r="O7" s="59">
         <v>0</v>
       </c>
       <c r="P7" s="1">
-        <v>149</v>
+        <v>299</v>
       </c>
       <c r="Q7" s="1">
         <v>300</v>
       </c>
+      <c r="R7" s="1">
+        <v>300</v>
+      </c>
       <c r="S7" s="1">
+        <v>300</v>
+      </c>
+      <c r="T7" s="1">
+        <v>300</v>
+      </c>
+      <c r="U7" s="38">
+        <v>300</v>
+      </c>
+      <c r="W7" s="1">
         <v>0</v>
       </c>
-      <c r="T7" s="1">
+      <c r="X7" s="1">
         <v>799</v>
       </c>
-      <c r="U7" s="1" t="s">
+      <c r="Y7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="V7" s="12">
+      <c r="Z7" s="12">
         <v>0.05</v>
       </c>
-      <c r="AA7" s="9"/>
-    </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AE7" s="9"/>
+    </row>
+    <row r="8" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="36">
-        <f>VLOOKUP(IF(C16,F7,F6),O7:Q21,3,TRUE)</f>
-        <v>280</v>
+        <f>VLOOKUP(IF(C16,F7,F6),Q17:S23,3)</f>
+        <v>300</v>
       </c>
       <c r="F8"/>
-      <c r="I8" s="50">
-        <v>3</v>
-      </c>
-      <c r="J8" s="50">
-        <f>2*NightTimeDrive5[[#This Row],[Time]]</f>
-        <v>6</v>
-      </c>
+      <c r="I8" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="57"/>
       <c r="L8" s="38" t="s">
         <v>49</v>
       </c>
       <c r="M8" s="30">
-        <v>254</v>
-      </c>
-      <c r="O8" s="1">
+        <v>220</v>
+      </c>
+      <c r="O8" s="59">
+        <v>300</v>
+      </c>
+      <c r="P8" s="1">
+        <v>599</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>100</v>
+      </c>
+      <c r="R8" s="1">
         <v>150</v>
       </c>
-      <c r="P8" s="1">
-        <v>299</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>280</v>
-      </c>
       <c r="S8" s="1">
+        <v>200</v>
+      </c>
+      <c r="T8" s="1">
+        <v>250</v>
+      </c>
+      <c r="U8" s="38">
+        <v>300</v>
+      </c>
+      <c r="W8" s="1">
         <v>800</v>
       </c>
-      <c r="T8" s="1">
+      <c r="X8" s="1">
         <v>1599</v>
       </c>
-      <c r="U8" s="1" t="s">
+      <c r="Y8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="V8" s="12">
+      <c r="Z8" s="12">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3088,111 +3469,156 @@
       <c r="G9" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="1">
+      <c r="L9" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="O9" s="59">
+        <v>600</v>
+      </c>
+      <c r="P9" s="1">
+        <v>899</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>75</v>
+      </c>
+      <c r="R9" s="1">
+        <v>150</v>
+      </c>
+      <c r="S9" s="1">
+        <v>200</v>
+      </c>
+      <c r="T9" s="1">
+        <v>250</v>
+      </c>
+      <c r="U9" s="38">
         <v>300</v>
       </c>
-      <c r="P9" s="1">
-        <v>449</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>260</v>
-      </c>
-      <c r="S9" s="1">
+      <c r="W9" s="1">
         <v>1600</v>
       </c>
-      <c r="T9" s="1">
+      <c r="X9" s="1">
         <v>2199</v>
       </c>
-      <c r="U9" s="1" t="s">
+      <c r="Y9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="V9" s="12">
+      <c r="Z9" s="12">
         <v>0.2</v>
       </c>
-      <c r="X9" s="9"/>
-    </row>
-    <row r="10" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AB9" s="9"/>
+    </row>
+    <row r="10" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="8">
         <f ca="1">SUM(C5:C9)</f>
-        <v>2566.25</v>
+        <v>2700</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>27</v>
       </c>
       <c r="F10" s="24">
-        <f ca="1">F6/M18</f>
-        <v>10.875</v>
+        <f ca="1">F6/M19</f>
+        <v>80.666666666666671</v>
       </c>
       <c r="G10" s="24">
-        <f ca="1">G6/M18</f>
-        <v>47.625</v>
-      </c>
-      <c r="L10" s="43" t="s">
+        <f ca="1">G6/M19</f>
+        <v>50</v>
+      </c>
+      <c r="I10" s="43" t="s">
+        <v>49</v>
+      </c>
+      <c r="J10" s="44"/>
+      <c r="O10" s="59">
+        <v>900</v>
+      </c>
+      <c r="P10" s="1">
+        <v>1199</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>50</v>
+      </c>
+      <c r="R10" s="1">
+        <v>100</v>
+      </c>
+      <c r="S10" s="1">
+        <v>150</v>
+      </c>
+      <c r="T10" s="1">
+        <v>200</v>
+      </c>
+      <c r="U10" s="38">
+        <v>300</v>
+      </c>
+      <c r="W10" s="1">
+        <v>2200</v>
+      </c>
+      <c r="X10" s="1">
+        <v>2499</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z10" s="12">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="I11" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="M10" s="44"/>
-      <c r="O10" s="1">
-        <v>450</v>
-      </c>
-      <c r="P10" s="1">
-        <v>599</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>240</v>
-      </c>
-      <c r="S10" s="1">
-        <v>2200</v>
-      </c>
-      <c r="T10" s="1">
-        <v>2499</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V10" s="12">
-        <v>0.35</v>
-      </c>
-    </row>
-    <row r="11" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="I11" s="9"/>
-      <c r="L11" s="39" t="s">
-        <v>56</v>
-      </c>
-      <c r="M11" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="O11" s="1">
-        <v>600</v>
+      <c r="M11" s="44"/>
+      <c r="O11" s="59">
+        <v>1200</v>
       </c>
       <c r="P11" s="1">
-        <v>749</v>
+        <v>1499</v>
       </c>
       <c r="Q11" s="1">
-        <v>220</v>
-      </c>
-      <c r="S11" s="5">
+        <v>25</v>
+      </c>
+      <c r="R11" s="1">
+        <v>75</v>
+      </c>
+      <c r="S11" s="1">
+        <v>100</v>
+      </c>
+      <c r="T11" s="1">
+        <v>175</v>
+      </c>
+      <c r="U11" s="38">
+        <v>300</v>
+      </c>
+      <c r="W11" s="5">
         <v>2500</v>
       </c>
-      <c r="T11" s="1">
+      <c r="X11" s="1">
         <v>3000</v>
       </c>
-      <c r="U11" s="1" t="s">
+      <c r="Y11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="V11" s="12">
+      <c r="Z11" s="12">
         <v>0.5</v>
       </c>
-      <c r="Y11"/>
-    </row>
-    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="AC11"/>
+    </row>
+    <row r="12" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C12" s="1" t="str">
-        <f ca="1">VLOOKUP(C10,S7:U11,3,TRUE)</f>
+        <f ca="1">VLOOKUP(C10,W7:Y11,3,TRUE)</f>
         <v>Diamond</v>
       </c>
       <c r="D12" s="9"/>
@@ -3203,118 +3629,144 @@
       <c r="G12" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="L12" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M12" s="41" t="s">
-        <v>54</v>
-      </c>
-      <c r="O12" s="1">
-        <v>750</v>
+      <c r="I12" s="52">
+        <v>0</v>
+      </c>
+      <c r="J12" s="52">
+        <f>2*NightTimeDrive55[[#This Row],[Time]]</f>
+        <v>0</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="O12" s="59">
+        <v>1500</v>
       </c>
       <c r="P12" s="1">
-        <v>899</v>
+        <v>1799</v>
       </c>
       <c r="Q12" s="1">
-        <v>200</v>
-      </c>
-      <c r="S12" s="6"/>
-      <c r="Y12" s="33"/>
-    </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="R12" s="1">
+        <v>25</v>
+      </c>
+      <c r="S12" s="1">
+        <v>50</v>
+      </c>
+      <c r="T12" s="1">
+        <v>100</v>
+      </c>
+      <c r="U12" s="38">
+        <v>250</v>
+      </c>
+      <c r="W12" s="6"/>
+      <c r="AC12" s="33"/>
+    </row>
+    <row r="13" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="35"/>
+      <c r="C13" s="35">
+        <v>0</v>
+      </c>
       <c r="E13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="25">
-        <f ca="1">IF(C8-M13&lt;=20, "Unlimited", INT(M13/20)*150 +VLOOKUP(F6,O7:Q21,2,TRUE) -F6)</f>
-        <v>488</v>
+      <c r="F13" s="25" t="str">
+        <f ca="1">IF(M24&gt;=P13, "Unlimited", M24-F6)</f>
+        <v>Unlimited</v>
       </c>
       <c r="G13" s="25">
-        <f ca="1">50*M19 + IF(M17&lt;30,(30-M17)*G10,0)</f>
-        <v>295.25</v>
+        <f ca="1">50*M20 + IF(M18&lt;30,(30-M18)*G10,0)</f>
+        <v>1250</v>
+      </c>
+      <c r="I13" s="53">
+        <v>0</v>
+      </c>
+      <c r="J13" s="53">
+        <f>2*NightTimeDrive55[[#This Row],[Time]]</f>
+        <v>0</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M13" s="1">
-        <f ca="1">C10-VLOOKUP(C10,S7:U11,1,TRUE)</f>
-        <v>66.25</v>
-      </c>
-      <c r="O13" s="1">
-        <v>900</v>
-      </c>
-      <c r="P13" s="1">
-        <v>1049</v>
-      </c>
-      <c r="Q13" s="1">
-        <v>180</v>
-      </c>
-      <c r="T13"/>
-      <c r="V13"/>
-      <c r="Y13" s="33"/>
-      <c r="Z13" s="9"/>
-    </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="M13" s="51" t="s">
+        <v>54</v>
+      </c>
+      <c r="O13" s="63">
+        <v>1800</v>
+      </c>
+      <c r="P13" s="42">
+        <v>1800</v>
+      </c>
+      <c r="Q13" s="42">
+        <v>5</v>
+      </c>
+      <c r="R13" s="42">
+        <v>10</v>
+      </c>
+      <c r="S13" s="42">
+        <v>25</v>
+      </c>
+      <c r="T13" s="42">
+        <v>60</v>
+      </c>
+      <c r="U13" s="64">
+        <v>100</v>
+      </c>
+      <c r="X13"/>
+      <c r="Z13"/>
+      <c r="AC13" s="33"/>
+      <c r="AD13" s="9"/>
+    </row>
+    <row r="14" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
         <v>1</v>
       </c>
       <c r="C14" s="8">
-        <f ca="1">C13*VLOOKUP(C12,U6:V11,2,FALSE)*10</f>
+        <f ca="1">C13*VLOOKUP(C12,Y6:Z11,2,FALSE)*10</f>
         <v>0</v>
       </c>
-      <c r="I14" s="9"/>
-      <c r="L14" s="38" t="s">
+      <c r="L14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" s="50">
+        <v>10</v>
+      </c>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+    </row>
+    <row r="15" spans="2:32" x14ac:dyDescent="0.25">
+      <c r="D15" s="14"/>
+      <c r="L15" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="M14" s="1">
-        <f>300-SUM(NightTimeDrive5[Points])</f>
-        <v>248</v>
-      </c>
-      <c r="O14" s="1">
-        <v>1050</v>
-      </c>
-      <c r="P14" s="1">
-        <v>1199</v>
-      </c>
-      <c r="Q14" s="1">
-        <v>160</v>
-      </c>
-      <c r="S14"/>
-      <c r="T14"/>
-      <c r="U14"/>
-      <c r="V14"/>
-      <c r="W14"/>
-    </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="D15" s="14"/>
-      <c r="L15" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="M15" s="1">
-        <v>2</v>
-      </c>
-      <c r="O15" s="1">
-        <v>1200</v>
-      </c>
-      <c r="P15" s="1">
-        <v>1349</v>
-      </c>
-      <c r="Q15" s="1">
-        <v>140</v>
-      </c>
-      <c r="S15"/>
-      <c r="T15"/>
-      <c r="U15" s="34"/>
-      <c r="V15"/>
+        <f>300-SUM(NightTimeDrive55[Points])</f>
+        <v>300</v>
+      </c>
+      <c r="Q15" s="58" t="str">
+        <f>_xlfn.CONCAT("Distance Points for ",M9)</f>
+        <v>Distance Points for Diamond</v>
+      </c>
+      <c r="R15" s="58"/>
+      <c r="S15" s="58"/>
       <c r="W15"/>
-      <c r="Z15" s="9"/>
-      <c r="AA15" s="9"/>
-    </row>
-    <row r="16" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="X15"/>
+      <c r="Y15" s="34"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+    </row>
+    <row r="16" spans="2:32" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>30</v>
       </c>
@@ -3322,336 +3774,380 @@
         <v>0</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M16" s="1" t="str">
-        <f>IF( AND( M8&lt;=M14+M15, M8&gt;=M14-M15 ), "Extract", "Calculate")</f>
+        <f>IF( AND( M8&lt;=M15+M14, M8&gt;=M15-M14 ), "Extract", "Calculate")</f>
         <v>Calculate</v>
       </c>
-      <c r="O16" s="1">
-        <v>1350</v>
-      </c>
-      <c r="P16" s="1">
-        <v>1499</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>120</v>
-      </c>
-      <c r="S16"/>
-      <c r="T16"/>
-      <c r="V16"/>
+      <c r="Q16" s="65" t="s">
+        <v>19</v>
+      </c>
+      <c r="R16" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="S16" s="65" t="s">
+        <v>17</v>
+      </c>
       <c r="W16"/>
-    </row>
-    <row r="17" spans="2:27" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-      <c r="F17" s="49"/>
-      <c r="G17" s="49"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="L17" s="1" t="str">
-        <f ca="1">_xlfn.CONCAT("Days ",TEXT(TODAY(), "mmmm 'yy"))</f>
-        <v>Days February '25</v>
-      </c>
-      <c r="M17" s="1">
+      <c r="X16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+    </row>
+    <row r="17" spans="2:31" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="54"/>
+      <c r="D17" s="54"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="54"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="32"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="Q17" s="66" cm="1">
+        <f t="array" ref="Q17:Q23">Table2[Lower]</f>
+        <v>0</v>
+      </c>
+      <c r="R17" s="66" cm="1">
+        <f t="array" ref="R17:R23">Table2[Upper]</f>
+        <v>299</v>
+      </c>
+      <c r="S17" s="66" cm="1">
+        <f t="array" ref="S17:S23">_xlfn.XLOOKUP(M9,Table2[#Headers],Table2[])</f>
+        <v>300</v>
+      </c>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+    </row>
+    <row r="18" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="54"/>
+      <c r="E18" s="54"/>
+      <c r="F18" s="54"/>
+      <c r="G18" s="54"/>
+      <c r="H18" s="32"/>
+      <c r="L18" s="1" t="str">
+        <f ca="1">_xlfn.CONCAT("Days ",TEXT(TODAY(), "mmm yyyy"))</f>
+        <v>Days Mar 2025</v>
+      </c>
+      <c r="M18" s="1">
         <f ca="1">DAY(EOMONTH(TODAY(), 0))</f>
-        <v>28</v>
-      </c>
-      <c r="O17" s="1">
-        <v>1500</v>
-      </c>
-      <c r="P17" s="1">
-        <v>1649</v>
-      </c>
-      <c r="Q17" s="1">
-        <v>100</v>
-      </c>
-      <c r="S17"/>
-      <c r="T17"/>
-      <c r="U17"/>
-      <c r="V17"/>
-      <c r="W17"/>
-    </row>
-    <row r="18" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B18" s="49"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
-      <c r="E18" s="49"/>
-      <c r="F18" s="49"/>
-      <c r="G18" s="49"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="49"/>
-      <c r="J18" s="49"/>
-      <c r="L18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M18" s="1">
+        <v>31</v>
+      </c>
+      <c r="Q18" s="66">
+        <v>300</v>
+      </c>
+      <c r="R18" s="66">
+        <v>599</v>
+      </c>
+      <c r="S18" s="66">
+        <v>300</v>
+      </c>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+    </row>
+    <row r="19" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="54"/>
+      <c r="G19" s="54"/>
+      <c r="H19" s="32"/>
+      <c r="L19" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M19" s="1">
         <f ca="1">DAY(TODAY())-1</f>
-        <v>24</v>
-      </c>
-      <c r="O18" s="1">
-        <v>1650</v>
-      </c>
-      <c r="P18" s="1">
-        <v>1799</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>80</v>
-      </c>
-      <c r="S18"/>
-      <c r="T18"/>
-      <c r="U18"/>
-      <c r="V18"/>
-      <c r="W18"/>
-    </row>
-    <row r="19" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="B19" s="32"/>
-      <c r="C19" s="32"/>
-      <c r="D19" s="32"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
-      <c r="I19" s="32"/>
-      <c r="J19" s="32"/>
-      <c r="L19" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="M19" s="1">
-        <f ca="1">M17-M18</f>
-        <v>4</v>
-      </c>
-      <c r="O19" s="1">
-        <v>1800</v>
-      </c>
-      <c r="P19" s="1">
-        <v>1949</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>60</v>
-      </c>
-      <c r="S19"/>
-      <c r="T19"/>
-      <c r="U19"/>
-      <c r="V19"/>
+        <v>6</v>
+      </c>
+      <c r="Q19" s="66">
+        <v>600</v>
+      </c>
+      <c r="R19" s="66">
+        <v>899</v>
+      </c>
+      <c r="S19" s="66">
+        <v>300</v>
+      </c>
       <c r="W19"/>
-    </row>
-    <row r="20" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+    </row>
+    <row r="20" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
       <c r="D20" s="32"/>
       <c r="E20" s="32"/>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
-      <c r="O20" s="1">
-        <v>1950</v>
-      </c>
-      <c r="P20" s="1">
-        <v>2099</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>40</v>
-      </c>
-      <c r="S20"/>
-      <c r="U20"/>
-      <c r="V20"/>
+      <c r="L20" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="M20" s="1">
+        <f ca="1">M18-M19</f>
+        <v>25</v>
+      </c>
+      <c r="Q20" s="66">
+        <v>900</v>
+      </c>
+      <c r="R20" s="66">
+        <v>1199</v>
+      </c>
+      <c r="S20" s="66">
+        <v>300</v>
+      </c>
       <c r="W20"/>
-    </row>
-    <row r="21" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+    </row>
+    <row r="21" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
       <c r="D21" s="32"/>
-      <c r="O21" s="1">
-        <v>2100</v>
-      </c>
-      <c r="P21" s="1">
-        <v>2100</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>20</v>
-      </c>
-      <c r="S21"/>
-      <c r="T21"/>
-      <c r="U21"/>
-      <c r="V21"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="Q21" s="66">
+        <v>1200</v>
+      </c>
+      <c r="R21" s="66">
+        <v>1499</v>
+      </c>
+      <c r="S21" s="66">
+        <v>300</v>
+      </c>
       <c r="W21"/>
-      <c r="Z21" s="9"/>
-      <c r="AA21" s="9"/>
-    </row>
-    <row r="22" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+    </row>
+    <row r="22" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
       <c r="D22" s="32"/>
-      <c r="W22"/>
-      <c r="Z22" s="9"/>
-      <c r="AA22" s="9"/>
-    </row>
-    <row r="23" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="L22" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M22" s="25">
+        <f ca="1">C10-VLOOKUP(C10,W7:Y11,1,TRUE)</f>
+        <v>200</v>
+      </c>
+      <c r="Q22" s="66">
+        <v>1500</v>
+      </c>
+      <c r="R22" s="66">
+        <v>1799</v>
+      </c>
+      <c r="S22" s="66">
+        <v>250</v>
+      </c>
+      <c r="AA22"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+    </row>
+    <row r="23" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B23" s="3"/>
-      <c r="S23"/>
-      <c r="T23"/>
-      <c r="U23"/>
-      <c r="V23"/>
+      <c r="L23" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M23" s="25">
+        <f ca="1">MAX(0,C8-M22)</f>
+        <v>100</v>
+      </c>
+      <c r="Q23" s="66">
+        <v>1800</v>
+      </c>
+      <c r="R23" s="66">
+        <v>1800</v>
+      </c>
+      <c r="S23" s="66">
+        <v>100</v>
+      </c>
       <c r="W23"/>
-    </row>
-    <row r="24" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="S24"/>
-      <c r="T24"/>
-      <c r="U24" s="21"/>
-      <c r="V24"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
+    </row>
+    <row r="24" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="L24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="M24" s="1" cm="1">
+        <f t="array" aca="1" ref="M24" ca="1">MAX(_xlfn._xlws.FILTER(_xlfn.ANCHORARRAY(R17),_xlfn.ANCHORARRAY( S17)&gt;=M23))</f>
+        <v>1800</v>
+      </c>
       <c r="W24"/>
-    </row>
-    <row r="25" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="S25"/>
-      <c r="T25"/>
-      <c r="U25" s="21"/>
-      <c r="V25"/>
+      <c r="X24"/>
+      <c r="Y24" s="21"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
+    </row>
+    <row r="25" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="U25" s="3"/>
       <c r="W25"/>
-    </row>
-    <row r="26" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="U26" s="2"/>
-    </row>
-    <row r="27" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="S27" s="6"/>
-      <c r="U27" s="2"/>
-    </row>
-    <row r="28" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="S28" s="6"/>
-      <c r="U28" s="2"/>
-    </row>
-    <row r="29" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="X25"/>
+      <c r="Y25" s="21"/>
+      <c r="Z25"/>
+      <c r="AA25"/>
+    </row>
+    <row r="26" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="Y26" s="2"/>
+    </row>
+    <row r="27" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="W27" s="6"/>
+      <c r="Y27" s="2"/>
+    </row>
+    <row r="28" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="I28" s="19"/>
+      <c r="J28" s="19"/>
+      <c r="W28" s="6"/>
+      <c r="Y28" s="2"/>
+    </row>
+    <row r="29" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
-      <c r="P29" s="4"/>
-      <c r="S29" s="6"/>
-      <c r="U29" s="2"/>
-    </row>
-    <row r="30" spans="2:27" x14ac:dyDescent="0.25">
-      <c r="S30" s="6"/>
-      <c r="U30" s="2"/>
-    </row>
-    <row r="31" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="W29" s="6"/>
+      <c r="Y29" s="2"/>
+    </row>
+    <row r="30" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="W30" s="6"/>
+      <c r="Y30" s="2"/>
+    </row>
+    <row r="31" spans="2:31" x14ac:dyDescent="0.25">
       <c r="E31" s="26"/>
       <c r="F31" s="26"/>
       <c r="G31" s="27"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="S31" s="6"/>
-      <c r="U31" s="2"/>
-    </row>
-    <row r="32" spans="2:27" x14ac:dyDescent="0.25">
+      <c r="W31" s="6"/>
+      <c r="Y31" s="2"/>
+    </row>
+    <row r="32" spans="2:31" x14ac:dyDescent="0.25">
       <c r="E32" s="26"/>
       <c r="F32" s="28"/>
       <c r="G32" s="27"/>
-      <c r="S32" s="6"/>
-      <c r="U32" s="2"/>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W32" s="6"/>
+      <c r="Y32" s="2"/>
+    </row>
+    <row r="33" spans="2:25" x14ac:dyDescent="0.25">
       <c r="E33" s="26"/>
       <c r="F33" s="28"/>
       <c r="G33" s="27"/>
-      <c r="S33" s="6"/>
-      <c r="U33" s="2"/>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W33" s="6"/>
+      <c r="Y33" s="2"/>
+    </row>
+    <row r="34" spans="2:25" x14ac:dyDescent="0.25">
       <c r="E34" s="26"/>
       <c r="F34" s="28"/>
       <c r="G34" s="27"/>
-      <c r="Q34" s="3"/>
-      <c r="S34" s="6"/>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="W34" s="6"/>
+    </row>
+    <row r="35" spans="2:25" x14ac:dyDescent="0.25">
       <c r="E35" s="26"/>
       <c r="F35" s="28"/>
       <c r="G35" s="27"/>
-      <c r="S35" s="6"/>
-    </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W35" s="6"/>
+    </row>
+    <row r="36" spans="2:25" x14ac:dyDescent="0.25">
       <c r="E36" s="26"/>
       <c r="F36" s="28"/>
       <c r="G36" s="27"/>
-      <c r="S36" s="6"/>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W36" s="6"/>
+    </row>
+    <row r="37" spans="2:25" x14ac:dyDescent="0.25">
       <c r="E37" s="26"/>
       <c r="F37" s="28"/>
       <c r="G37" s="27"/>
-      <c r="S37" s="6"/>
-    </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W37" s="6"/>
+    </row>
+    <row r="38" spans="2:25" x14ac:dyDescent="0.25">
       <c r="E38" s="26"/>
       <c r="F38" s="28"/>
       <c r="G38" s="27"/>
-      <c r="L38" s="19"/>
-      <c r="M38" s="19"/>
-      <c r="S38" s="6"/>
-    </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W38" s="6"/>
+    </row>
+    <row r="39" spans="2:25" x14ac:dyDescent="0.25">
       <c r="E39" s="26"/>
       <c r="F39" s="28"/>
       <c r="G39" s="29"/>
-      <c r="S39" s="6"/>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W39" s="6"/>
+    </row>
+    <row r="40" spans="2:25" x14ac:dyDescent="0.25">
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:25" x14ac:dyDescent="0.25">
       <c r="H41" s="19"/>
       <c r="K41" s="19"/>
       <c r="N41" s="19"/>
-      <c r="S41" s="6"/>
-    </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="W41" s="6"/>
+    </row>
+    <row r="42" spans="2:25" x14ac:dyDescent="0.25">
       <c r="B42" s="19"/>
-      <c r="S42" s="6"/>
-    </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="S43" s="6"/>
-    </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="O44" s="3"/>
-      <c r="S44" s="6"/>
-    </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="S45" s="6"/>
-    </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="S46" s="6"/>
-    </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="S47" s="6"/>
-    </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="S48" s="6"/>
-    </row>
-    <row r="49" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S49" s="6"/>
-    </row>
-    <row r="50" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S50" s="6"/>
+      <c r="W42" s="6"/>
+    </row>
+    <row r="43" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W43" s="6"/>
+    </row>
+    <row r="44" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W44" s="6"/>
+    </row>
+    <row r="45" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W45" s="6"/>
+    </row>
+    <row r="46" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W46" s="6"/>
+    </row>
+    <row r="47" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W47" s="6"/>
+    </row>
+    <row r="48" spans="2:25" x14ac:dyDescent="0.25">
+      <c r="W48" s="6"/>
+    </row>
+    <row r="49" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W49" s="6"/>
+    </row>
+    <row r="50" spans="23:23" x14ac:dyDescent="0.25">
+      <c r="W50" s="6"/>
     </row>
   </sheetData>
   <protectedRanges>
-    <protectedRange sqref="F6:G6 C6:C7 C9 C13" name="RequiresInput"/>
+    <protectedRange sqref="F6:G6 C6:C7 C9 C13" name="RequiresInput_1"/>
   </protectedRanges>
-  <mergeCells count="8">
-    <mergeCell ref="B17:J18"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="L10:M10"/>
+  <mergeCells count="13">
+    <mergeCell ref="B17:G19"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="AE5:AF5"/>
     <mergeCell ref="B2:J3"/>
-    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="L5:M5"/>
-    <mergeCell ref="O5:Q5"/>
-    <mergeCell ref="S5:V5"/>
+    <mergeCell ref="W5:Z5"/>
+    <mergeCell ref="L11:M11"/>
+    <mergeCell ref="O5:U5"/>
+    <mergeCell ref="Q15:S15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>